<commit_message>
Test-NMSW-1233 Duplication record across FAl5 and 6
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Fal6-Files/FAL 6-With-same-TD-NumberAndCountry-asFAL5.xlsx
+++ b/cypress/fixtures/Fal6-Files/FAL 6-With-same-TD-NumberAndCountry-asFAL5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSW-Main\nmsw-ui\cypress\fixtures\Fal6-Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSWTemp\nmsw-ui\cypress\fixtures\Fal6-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91E89B9-BEF0-4F45-922B-4E4D8F73AA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F72A96-B35F-469A-B15F-A56DA1AFE329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FAL 6" sheetId="1" r:id="rId1"/>
@@ -5045,17 +5045,17 @@
     <t>GB NCL</t>
   </si>
   <si>
-    <t xml:space="preserve">Younger                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adam                                    </t>
+    <t>Alfred</t>
+  </si>
+  <si>
+    <t>JB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -5165,6 +5165,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -5755,7 +5762,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -5964,6 +5971,9 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="7" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -7131,23 +7141,23 @@
   <dimension ref="A1:P977"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="4" width="19.81640625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" style="14" customWidth="1"/>
-    <col min="6" max="11" width="19.81640625" style="14" customWidth="1"/>
-    <col min="12" max="12" width="20.1796875" style="14" customWidth="1"/>
-    <col min="13" max="13" width="19.81640625" style="14" customWidth="1"/>
-    <col min="14" max="14" width="22.453125" style="14" customWidth="1"/>
-    <col min="15" max="15" width="20.453125" style="14" customWidth="1"/>
-    <col min="16" max="16" width="14.453125" style="14" hidden="1" customWidth="1"/>
+    <col min="1" max="4" width="19.85546875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="14" customWidth="1"/>
+    <col min="6" max="11" width="19.85546875" style="14" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" style="14" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" style="14" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" style="14" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" style="14" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" style="14" hidden="1" customWidth="1"/>
     <col min="17" max="16384" width="0" style="14" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="13" customFormat="1" ht="93">
+    <row r="1" spans="1:16" s="13" customFormat="1" ht="94.5">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -7185,7 +7195,7 @@
       <c r="N2" s="57"/>
       <c r="O2" s="58"/>
     </row>
-    <row r="3" spans="1:16" ht="62">
+    <row r="3" spans="1:16" ht="63">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
@@ -7232,7 +7242,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="40" customFormat="1" ht="201.5">
+    <row r="4" spans="1:16" s="40" customFormat="1" ht="195">
       <c r="A4" s="35" t="s">
         <v>17</v>
       </c>
@@ -7279,7 +7289,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" ht="15">
       <c r="A5" s="17" t="s">
         <v>1632</v>
       </c>
@@ -7324,7 +7334,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" ht="15">
       <c r="A6" s="48" t="s">
         <v>1632</v>
       </c>
@@ -7369,7 +7379,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" ht="15">
       <c r="A7" s="48" t="s">
         <v>1632</v>
       </c>
@@ -7380,7 +7390,7 @@
       <c r="D7" s="49">
         <v>123456789</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="71" t="s">
         <v>1646</v>
       </c>
       <c r="F7" s="48" t="s">
@@ -7414,7 +7424,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" ht="15">
       <c r="A8" s="20"/>
       <c r="B8" s="21"/>
       <c r="C8" s="20"/>
@@ -7431,7 +7441,7 @@
       <c r="N8" s="20"/>
       <c r="O8" s="20"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" ht="15">
       <c r="A9" s="20"/>
       <c r="B9" s="21"/>
       <c r="C9" s="20"/>
@@ -7448,7 +7458,7 @@
       <c r="N9" s="20"/>
       <c r="O9" s="20"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" ht="15">
       <c r="A10" s="20"/>
       <c r="B10" s="21"/>
       <c r="C10" s="20"/>
@@ -7465,7 +7475,7 @@
       <c r="N10" s="20"/>
       <c r="O10" s="20"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" ht="15">
       <c r="A11" s="20"/>
       <c r="B11" s="21"/>
       <c r="C11" s="20"/>
@@ -7482,7 +7492,7 @@
       <c r="N11" s="20"/>
       <c r="O11" s="20"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" ht="15">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
       <c r="C12" s="20"/>
@@ -7499,7 +7509,7 @@
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" ht="15">
       <c r="A13" s="23"/>
       <c r="B13" s="24"/>
       <c r="C13" s="23"/>
@@ -7516,7 +7526,7 @@
       <c r="N13" s="23"/>
       <c r="O13" s="23"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" ht="15">
       <c r="A14" s="26"/>
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
@@ -7534,7 +7544,7 @@
       <c r="O14" s="26"/>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" ht="15">
       <c r="A15" s="28"/>
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
@@ -7552,7 +7562,7 @@
       <c r="O15" s="28"/>
       <c r="P15" s="27"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" ht="15">
       <c r="A16" s="26"/>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
@@ -7570,7 +7580,7 @@
       <c r="O16" s="26"/>
       <c r="P16" s="27"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" ht="15">
       <c r="A17" s="26"/>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
@@ -7588,7 +7598,7 @@
       <c r="O17" s="26"/>
       <c r="P17" s="27"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" ht="15">
       <c r="A18" s="26"/>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -7606,7 +7616,7 @@
       <c r="O18" s="26"/>
       <c r="P18" s="27"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" ht="15">
       <c r="A19" s="26"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
@@ -7624,7 +7634,7 @@
       <c r="O19" s="26"/>
       <c r="P19" s="27"/>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" ht="15">
       <c r="A20" s="26"/>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -23954,15 +23964,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="42"/>
-    <col min="2" max="2" width="9.453125" style="42" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="42"/>
+    <col min="2" max="2" width="9.42578125" style="42" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="58.5">
@@ -23970,7 +23980,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.5">
+    <row r="2" spans="1:7" ht="15.75">
       <c r="A2" s="43" t="s">
         <v>33</v>
       </c>
@@ -23993,7 +24003,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.5">
+    <row r="3" spans="1:7" ht="15.75">
       <c r="A3" s="42" t="s">
         <v>40</v>
       </c>
@@ -24016,7 +24026,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.5">
+    <row r="4" spans="1:7" ht="15.75">
       <c r="A4" s="42" t="s">
         <v>47</v>
       </c>
@@ -24039,7 +24049,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.5">
+    <row r="5" spans="1:7" ht="15.75">
       <c r="A5" s="42" t="s">
         <v>53</v>
       </c>
@@ -24062,7 +24072,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.5">
+    <row r="6" spans="1:7" ht="15.75">
       <c r="A6" s="42" t="s">
         <v>59</v>
       </c>
@@ -24085,7 +24095,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.5">
+    <row r="7" spans="1:7" ht="15.75">
       <c r="A7" s="42" t="s">
         <v>65</v>
       </c>
@@ -24108,7 +24118,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.5">
+    <row r="8" spans="1:7" ht="15.75">
       <c r="A8" s="42" t="s">
         <v>71</v>
       </c>
@@ -24131,7 +24141,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.5">
+    <row r="9" spans="1:7" ht="15.75">
       <c r="A9" s="42" t="s">
         <v>77</v>
       </c>
@@ -24154,7 +24164,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.5">
+    <row r="10" spans="1:7" ht="15.75">
       <c r="A10" s="42" t="s">
         <v>83</v>
       </c>
@@ -24177,7 +24187,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.5">
+    <row r="11" spans="1:7" ht="15.75">
       <c r="A11" s="42" t="s">
         <v>90</v>
       </c>
@@ -24200,7 +24210,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.5">
+    <row r="12" spans="1:7" ht="15.75">
       <c r="A12" s="42" t="s">
         <v>97</v>
       </c>
@@ -24223,7 +24233,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.5">
+    <row r="13" spans="1:7" ht="15.75">
       <c r="A13" s="42" t="s">
         <v>103</v>
       </c>
@@ -24246,7 +24256,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.5">
+    <row r="14" spans="1:7" ht="15.75">
       <c r="A14" s="42" t="s">
         <v>109</v>
       </c>
@@ -24269,7 +24279,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.5">
+    <row r="15" spans="1:7" ht="15.75">
       <c r="A15" s="42" t="s">
         <v>115</v>
       </c>
@@ -24292,7 +24302,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.5">
+    <row r="16" spans="1:7" ht="15.75">
       <c r="A16" s="42" t="s">
         <v>122</v>
       </c>
@@ -24315,7 +24325,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.5">
+    <row r="17" spans="1:7" ht="15.75">
       <c r="A17" s="42" t="s">
         <v>128</v>
       </c>
@@ -24338,7 +24348,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.5">
+    <row r="18" spans="1:7" ht="15.75">
       <c r="A18" s="42" t="s">
         <v>134</v>
       </c>
@@ -24361,7 +24371,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.5">
+    <row r="19" spans="1:7" ht="15.75">
       <c r="A19" s="42" t="s">
         <v>140</v>
       </c>
@@ -24384,7 +24394,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.5">
+    <row r="20" spans="1:7" ht="15.75">
       <c r="A20" s="42" t="s">
         <v>146</v>
       </c>
@@ -24407,7 +24417,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.5">
+    <row r="21" spans="1:7" ht="15.75">
       <c r="A21" s="42" t="s">
         <v>153</v>
       </c>
@@ -24430,7 +24440,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.5">
+    <row r="22" spans="1:7" ht="15.75">
       <c r="A22" s="42" t="s">
         <v>160</v>
       </c>
@@ -24453,7 +24463,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.5">
+    <row r="23" spans="1:7" ht="15.75">
       <c r="A23" s="42" t="s">
         <v>166</v>
       </c>
@@ -24476,7 +24486,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.5">
+    <row r="24" spans="1:7" ht="15.75">
       <c r="A24" s="42" t="s">
         <v>172</v>
       </c>
@@ -24499,7 +24509,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.5">
+    <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="42" t="s">
         <v>178</v>
       </c>
@@ -24522,7 +24532,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.5">
+    <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="42" t="s">
         <v>184</v>
       </c>
@@ -24545,7 +24555,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.5">
+    <row r="27" spans="1:7" ht="15.75">
       <c r="A27" s="42" t="s">
         <v>190</v>
       </c>
@@ -24568,7 +24578,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.5">
+    <row r="28" spans="1:7" ht="15.75">
       <c r="A28" s="42" t="s">
         <v>197</v>
       </c>
@@ -24591,7 +24601,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.5">
+    <row r="29" spans="1:7" ht="15.75">
       <c r="A29" s="42" t="s">
         <v>203</v>
       </c>
@@ -24614,7 +24624,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.5">
+    <row r="30" spans="1:7" ht="15.75">
       <c r="A30" s="42" t="s">
         <v>209</v>
       </c>
@@ -24637,7 +24647,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.5">
+    <row r="31" spans="1:7" ht="15.75">
       <c r="A31" s="42" t="s">
         <v>215</v>
       </c>
@@ -24660,7 +24670,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.5">
+    <row r="32" spans="1:7" ht="15.75">
       <c r="A32" s="42" t="s">
         <v>222</v>
       </c>
@@ -24683,7 +24693,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.5">
+    <row r="33" spans="1:7" ht="15.75">
       <c r="A33" s="42" t="s">
         <v>229</v>
       </c>
@@ -24706,7 +24716,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.5">
+    <row r="34" spans="1:7" ht="15.75">
       <c r="A34" s="42" t="s">
         <v>236</v>
       </c>
@@ -24729,7 +24739,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.5">
+    <row r="35" spans="1:7" ht="15.75">
       <c r="A35" s="42" t="s">
         <v>243</v>
       </c>
@@ -24752,7 +24762,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.5">
+    <row r="36" spans="1:7" ht="15.75">
       <c r="A36" s="42" t="s">
         <v>249</v>
       </c>
@@ -24775,7 +24785,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.5">
+    <row r="37" spans="1:7" ht="15.75">
       <c r="A37" s="42" t="s">
         <v>255</v>
       </c>
@@ -24798,7 +24808,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.5">
+    <row r="38" spans="1:7" ht="15.75">
       <c r="A38" s="42" t="s">
         <v>261</v>
       </c>
@@ -24821,7 +24831,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.5">
+    <row r="39" spans="1:7" ht="15.75">
       <c r="A39" s="42" t="s">
         <v>267</v>
       </c>
@@ -24844,7 +24854,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.5">
+    <row r="40" spans="1:7" ht="15.75">
       <c r="A40" s="42" t="s">
         <v>273</v>
       </c>
@@ -24867,7 +24877,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.5">
+    <row r="41" spans="1:7" ht="15.75">
       <c r="A41" s="42" t="s">
         <v>279</v>
       </c>
@@ -24890,7 +24900,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15.5">
+    <row r="42" spans="1:7" ht="15.75">
       <c r="A42" s="42" t="s">
         <v>286</v>
       </c>
@@ -24913,7 +24923,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15.5">
+    <row r="43" spans="1:7" ht="15.75">
       <c r="A43" s="42" t="s">
         <v>293</v>
       </c>
@@ -24936,7 +24946,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15.5">
+    <row r="44" spans="1:7" ht="15.75">
       <c r="A44" s="42" t="s">
         <v>299</v>
       </c>
@@ -24959,7 +24969,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15.5">
+    <row r="45" spans="1:7" ht="15.75">
       <c r="A45" s="42" t="s">
         <v>305</v>
       </c>
@@ -24982,7 +24992,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15.5">
+    <row r="46" spans="1:7" ht="15.75">
       <c r="A46" s="42" t="s">
         <v>311</v>
       </c>
@@ -25005,7 +25015,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15.5">
+    <row r="47" spans="1:7" ht="15.75">
       <c r="A47" s="42" t="s">
         <v>318</v>
       </c>
@@ -25028,7 +25038,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15.5">
+    <row r="48" spans="1:7" ht="15.75">
       <c r="A48" s="42" t="s">
         <v>324</v>
       </c>
@@ -25051,7 +25061,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15.5">
+    <row r="49" spans="1:7" ht="15.75">
       <c r="A49" s="42" t="s">
         <v>330</v>
       </c>
@@ -25074,7 +25084,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15.5">
+    <row r="50" spans="1:7" ht="15.75">
       <c r="A50" s="42" t="s">
         <v>336</v>
       </c>
@@ -25097,7 +25107,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15.5">
+    <row r="51" spans="1:7" ht="15.75">
       <c r="A51" s="42" t="s">
         <v>342</v>
       </c>
@@ -25120,7 +25130,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15.5">
+    <row r="52" spans="1:7" ht="15.75">
       <c r="A52" s="42" t="s">
         <v>349</v>
       </c>
@@ -25143,7 +25153,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15.5">
+    <row r="53" spans="1:7" ht="15.75">
       <c r="A53" s="42" t="s">
         <v>356</v>
       </c>
@@ -25166,7 +25176,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15.5">
+    <row r="54" spans="1:7" ht="15.75">
       <c r="A54" s="42" t="s">
         <v>362</v>
       </c>
@@ -25189,7 +25199,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15.5">
+    <row r="55" spans="1:7" ht="15.75">
       <c r="A55" s="42" t="s">
         <v>368</v>
       </c>
@@ -25212,7 +25222,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15.5">
+    <row r="56" spans="1:7" ht="15.75">
       <c r="A56" s="42" t="s">
         <v>374</v>
       </c>
@@ -25235,7 +25245,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15.5">
+    <row r="57" spans="1:7" ht="15.75">
       <c r="A57" s="42" t="s">
         <v>380</v>
       </c>
@@ -25258,7 +25268,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15.5">
+    <row r="58" spans="1:7" ht="15.75">
       <c r="A58" s="42" t="s">
         <v>386</v>
       </c>
@@ -25281,7 +25291,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="15.5">
+    <row r="59" spans="1:7" ht="15.75">
       <c r="A59" s="42" t="s">
         <v>393</v>
       </c>
@@ -25304,7 +25314,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15.5">
+    <row r="60" spans="1:7" ht="15.75">
       <c r="A60" s="42" t="s">
         <v>399</v>
       </c>
@@ -25327,7 +25337,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="15.5">
+    <row r="61" spans="1:7" ht="15.75">
       <c r="A61" s="42" t="s">
         <v>405</v>
       </c>
@@ -25350,7 +25360,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15.5">
+    <row r="62" spans="1:7" ht="15.75">
       <c r="A62" s="42" t="s">
         <v>411</v>
       </c>
@@ -25373,7 +25383,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="15.5">
+    <row r="63" spans="1:7" ht="15.75">
       <c r="A63" s="42" t="s">
         <v>418</v>
       </c>
@@ -25396,7 +25406,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15.5">
+    <row r="64" spans="1:7" ht="15.75">
       <c r="A64" s="42" t="s">
         <v>425</v>
       </c>
@@ -25419,7 +25429,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15.5">
+    <row r="65" spans="1:7" ht="15.75">
       <c r="A65" s="42" t="s">
         <v>431</v>
       </c>
@@ -25442,7 +25452,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15.5">
+    <row r="66" spans="1:7" ht="15.75">
       <c r="A66" s="42" t="s">
         <v>437</v>
       </c>
@@ -25465,7 +25475,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15.5">
+    <row r="67" spans="1:7" ht="15.75">
       <c r="A67" s="42" t="s">
         <v>443</v>
       </c>
@@ -25488,7 +25498,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15.5">
+    <row r="68" spans="1:7" ht="15.75">
       <c r="A68" s="42" t="s">
         <v>448</v>
       </c>
@@ -25511,7 +25521,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15.5">
+    <row r="69" spans="1:7" ht="15.75">
       <c r="A69" s="42" t="s">
         <v>453</v>
       </c>
@@ -25534,7 +25544,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15.5">
+    <row r="70" spans="1:7" ht="15.75">
       <c r="A70" s="42" t="s">
         <v>458</v>
       </c>
@@ -25557,7 +25567,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15.5">
+    <row r="71" spans="1:7" ht="15.75">
       <c r="A71" s="42" t="s">
         <v>463</v>
       </c>
@@ -25580,7 +25590,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15.5">
+    <row r="72" spans="1:7" ht="15.75">
       <c r="A72" s="42" t="s">
         <v>469</v>
       </c>
@@ -25603,7 +25613,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15.5">
+    <row r="73" spans="1:7" ht="15.75">
       <c r="A73" s="42" t="s">
         <v>475</v>
       </c>
@@ -25626,7 +25636,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15.5">
+    <row r="74" spans="1:7" ht="15.75">
       <c r="A74" s="42" t="s">
         <v>481</v>
       </c>
@@ -25649,7 +25659,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15.5">
+    <row r="75" spans="1:7" ht="15.75">
       <c r="A75" s="42" t="s">
         <v>487</v>
       </c>
@@ -25672,7 +25682,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15.5">
+    <row r="76" spans="1:7" ht="15.75">
       <c r="A76" s="42" t="s">
         <v>493</v>
       </c>
@@ -25695,7 +25705,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15.5">
+    <row r="77" spans="1:7" ht="15.75">
       <c r="A77" s="42" t="s">
         <v>499</v>
       </c>
@@ -25718,7 +25728,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15.5">
+    <row r="78" spans="1:7" ht="15.75">
       <c r="A78" s="42" t="s">
         <v>504</v>
       </c>
@@ -25741,7 +25751,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15.5">
+    <row r="79" spans="1:7" ht="15.75">
       <c r="A79" s="42" t="s">
         <v>509</v>
       </c>
@@ -25764,7 +25774,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15.5">
+    <row r="80" spans="1:7" ht="15.75">
       <c r="A80" s="42" t="s">
         <v>516</v>
       </c>
@@ -25787,7 +25797,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15.5">
+    <row r="81" spans="1:7" ht="15.75">
       <c r="A81" s="42" t="s">
         <v>523</v>
       </c>
@@ -25810,7 +25820,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15.5">
+    <row r="82" spans="1:7" ht="15.75">
       <c r="A82" s="42" t="s">
         <v>528</v>
       </c>
@@ -25833,7 +25843,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15.5">
+    <row r="83" spans="1:7" ht="15.75">
       <c r="A83" s="42" t="s">
         <v>533</v>
       </c>
@@ -25856,7 +25866,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15.5">
+    <row r="84" spans="1:7" ht="15.75">
       <c r="A84" s="42" t="s">
         <v>538</v>
       </c>
@@ -25879,7 +25889,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15.5">
+    <row r="85" spans="1:7" ht="15.75">
       <c r="A85" s="42" t="s">
         <v>543</v>
       </c>
@@ -25902,7 +25912,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15.5">
+    <row r="86" spans="1:7" ht="15.75">
       <c r="A86" s="42" t="s">
         <v>548</v>
       </c>
@@ -25925,7 +25935,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15.5">
+    <row r="87" spans="1:7" ht="15.75">
       <c r="A87" s="42" t="s">
         <v>553</v>
       </c>
@@ -25948,7 +25958,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15.5">
+    <row r="88" spans="1:7" ht="15.75">
       <c r="A88" s="42" t="s">
         <v>558</v>
       </c>
@@ -25971,7 +25981,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15.5">
+    <row r="89" spans="1:7" ht="15.75">
       <c r="A89" s="42" t="s">
         <v>563</v>
       </c>
@@ -25994,7 +26004,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15.5">
+    <row r="90" spans="1:7" ht="15.75">
       <c r="A90" s="42" t="s">
         <v>568</v>
       </c>
@@ -26017,7 +26027,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15.5">
+    <row r="91" spans="1:7" ht="15.75">
       <c r="A91" s="42" t="s">
         <v>573</v>
       </c>
@@ -26040,7 +26050,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="15.5">
+    <row r="92" spans="1:7" ht="15.75">
       <c r="A92" s="42" t="s">
         <v>580</v>
       </c>
@@ -26063,7 +26073,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15.5">
+    <row r="93" spans="1:7" ht="15.75">
       <c r="A93" s="42" t="s">
         <v>587</v>
       </c>
@@ -26086,7 +26096,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="15.5">
+    <row r="94" spans="1:7" ht="15.75">
       <c r="A94" s="42" t="s">
         <v>593</v>
       </c>
@@ -26109,7 +26119,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15.5">
+    <row r="95" spans="1:7" ht="15.75">
       <c r="A95" s="42" t="s">
         <v>599</v>
       </c>
@@ -26132,7 +26142,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15.5">
+    <row r="96" spans="1:7" ht="15.75">
       <c r="A96" s="42" t="s">
         <v>604</v>
       </c>
@@ -26155,7 +26165,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15.5">
+    <row r="97" spans="1:7" ht="15.75">
       <c r="A97" s="42" t="s">
         <v>609</v>
       </c>
@@ -26178,7 +26188,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15.5">
+    <row r="98" spans="1:7" ht="15.75">
       <c r="A98" s="42" t="s">
         <v>615</v>
       </c>
@@ -26201,7 +26211,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15.5">
+    <row r="99" spans="1:7" ht="15.75">
       <c r="A99" s="42" t="s">
         <v>622</v>
       </c>
@@ -26224,7 +26234,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15.5">
+    <row r="100" spans="1:7" ht="15.75">
       <c r="A100" s="42" t="s">
         <v>629</v>
       </c>
@@ -26247,7 +26257,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15.5">
+    <row r="101" spans="1:7" ht="15.75">
       <c r="A101" s="42" t="s">
         <v>635</v>
       </c>
@@ -26270,7 +26280,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="15.5">
+    <row r="102" spans="1:7" ht="15.75">
       <c r="A102" s="42" t="s">
         <v>641</v>
       </c>
@@ -26293,7 +26303,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="15.5">
+    <row r="103" spans="1:7" ht="15.75">
       <c r="A103" s="42" t="s">
         <v>648</v>
       </c>
@@ -26316,7 +26326,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="15.5">
+    <row r="104" spans="1:7" ht="15.75">
       <c r="A104" s="42" t="s">
         <v>654</v>
       </c>
@@ -26339,7 +26349,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15.5">
+    <row r="105" spans="1:7" ht="15.75">
       <c r="A105" s="42" t="s">
         <v>660</v>
       </c>
@@ -26362,7 +26372,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="15.5">
+    <row r="106" spans="1:7" ht="15.75">
       <c r="A106" s="42" t="s">
         <v>666</v>
       </c>
@@ -26385,7 +26395,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="15.5">
+    <row r="107" spans="1:7" ht="15.75">
       <c r="A107" s="42" t="s">
         <v>671</v>
       </c>
@@ -26408,7 +26418,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="15.5">
+    <row r="108" spans="1:7" ht="15.75">
       <c r="A108" s="42" t="s">
         <v>676</v>
       </c>
@@ -26431,7 +26441,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="15.5">
+    <row r="109" spans="1:7" ht="15.75">
       <c r="A109" s="42" t="s">
         <v>681</v>
       </c>
@@ -26454,7 +26464,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="15.5">
+    <row r="110" spans="1:7" ht="15.75">
       <c r="A110" s="42" t="s">
         <v>687</v>
       </c>
@@ -26477,7 +26487,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="15.5">
+    <row r="111" spans="1:7" ht="15.75">
       <c r="A111" s="42" t="s">
         <v>692</v>
       </c>
@@ -26500,7 +26510,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="15.5">
+    <row r="112" spans="1:7" ht="15.75">
       <c r="A112" s="42" t="s">
         <v>697</v>
       </c>
@@ -26523,7 +26533,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="15.5">
+    <row r="113" spans="1:7" ht="15.75">
       <c r="A113" s="42" t="s">
         <v>704</v>
       </c>
@@ -26546,7 +26556,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="15.5">
+    <row r="114" spans="1:7" ht="15.75">
       <c r="A114" s="42" t="s">
         <v>711</v>
       </c>
@@ -26569,7 +26579,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="15.5">
+    <row r="115" spans="1:7" ht="15.75">
       <c r="A115" s="42" t="s">
         <v>718</v>
       </c>
@@ -26592,7 +26602,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="15.5">
+    <row r="116" spans="1:7" ht="15.75">
       <c r="A116" s="42" t="s">
         <v>725</v>
       </c>
@@ -26615,7 +26625,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="15.5">
+    <row r="117" spans="1:7" ht="15.75">
       <c r="A117" s="42" t="s">
         <v>731</v>
       </c>
@@ -26638,7 +26648,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="15.5">
+    <row r="118" spans="1:7" ht="15.75">
       <c r="A118" s="42" t="s">
         <v>738</v>
       </c>
@@ -26661,7 +26671,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="15.5">
+    <row r="119" spans="1:7" ht="15.75">
       <c r="A119" s="42" t="s">
         <v>744</v>
       </c>
@@ -26684,7 +26694,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="15.5">
+    <row r="120" spans="1:7" ht="15.75">
       <c r="A120" s="42" t="s">
         <v>750</v>
       </c>
@@ -26707,7 +26717,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="15.5">
+    <row r="121" spans="1:7" ht="15.75">
       <c r="A121" s="42" t="s">
         <v>756</v>
       </c>
@@ -26730,7 +26740,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="15.5">
+    <row r="122" spans="1:7" ht="15.75">
       <c r="A122" s="42" t="s">
         <v>762</v>
       </c>
@@ -26753,7 +26763,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="15.5">
+    <row r="123" spans="1:7" ht="15.75">
       <c r="A123" s="42" t="s">
         <v>767</v>
       </c>
@@ -26776,7 +26786,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="15.5">
+    <row r="124" spans="1:7" ht="15.75">
       <c r="A124" s="42" t="s">
         <v>772</v>
       </c>
@@ -26799,7 +26809,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="15.5">
+    <row r="125" spans="1:7" ht="15.75">
       <c r="A125" s="42" t="s">
         <v>777</v>
       </c>
@@ -26822,7 +26832,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="15.5">
+    <row r="126" spans="1:7" ht="15.75">
       <c r="A126" s="42" t="s">
         <v>782</v>
       </c>
@@ -26845,7 +26855,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="15.5">
+    <row r="127" spans="1:7" ht="15.75">
       <c r="A127" s="42" t="s">
         <v>788</v>
       </c>
@@ -26868,7 +26878,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="15.5">
+    <row r="128" spans="1:7" ht="15.75">
       <c r="A128" s="42" t="s">
         <v>794</v>
       </c>
@@ -26891,7 +26901,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="15.5">
+    <row r="129" spans="1:7" ht="15.75">
       <c r="A129" s="42" t="s">
         <v>800</v>
       </c>
@@ -26914,7 +26924,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="15.5">
+    <row r="130" spans="1:7" ht="15.75">
       <c r="A130" s="42" t="s">
         <v>806</v>
       </c>
@@ -26937,7 +26947,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="15.5">
+    <row r="131" spans="1:7" ht="15.75">
       <c r="A131" s="42" t="s">
         <v>812</v>
       </c>
@@ -26960,7 +26970,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="15.5">
+    <row r="132" spans="1:7" ht="15.75">
       <c r="A132" s="42" t="s">
         <v>818</v>
       </c>
@@ -26983,7 +26993,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="15.5">
+    <row r="133" spans="1:7" ht="15.75">
       <c r="A133" s="42" t="s">
         <v>823</v>
       </c>
@@ -27006,7 +27016,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="15.5">
+    <row r="134" spans="1:7" ht="15.75">
       <c r="A134" s="42" t="s">
         <v>829</v>
       </c>
@@ -27029,7 +27039,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="15.5">
+    <row r="135" spans="1:7" ht="15.75">
       <c r="A135" s="42" t="s">
         <v>835</v>
       </c>
@@ -27052,7 +27062,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="15.5">
+    <row r="136" spans="1:7" ht="15.75">
       <c r="A136" s="42" t="s">
         <v>840</v>
       </c>
@@ -27075,7 +27085,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="15.5">
+    <row r="137" spans="1:7" ht="15.75">
       <c r="A137" s="42" t="s">
         <v>845</v>
       </c>
@@ -27098,7 +27108,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="15.5">
+    <row r="138" spans="1:7" ht="15.75">
       <c r="A138" s="42" t="s">
         <v>850</v>
       </c>
@@ -27121,7 +27131,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="15.5">
+    <row r="139" spans="1:7" ht="15.75">
       <c r="A139" s="42" t="s">
         <v>855</v>
       </c>
@@ -27144,7 +27154,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="15.5">
+    <row r="140" spans="1:7" ht="15.75">
       <c r="A140" s="42" t="s">
         <v>861</v>
       </c>
@@ -27167,7 +27177,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="15.5">
+    <row r="141" spans="1:7" ht="15.75">
       <c r="A141" s="42" t="s">
         <v>867</v>
       </c>
@@ -27190,7 +27200,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="15.5">
+    <row r="142" spans="1:7" ht="15.75">
       <c r="A142" s="42" t="s">
         <v>874</v>
       </c>
@@ -27213,7 +27223,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="15.5">
+    <row r="143" spans="1:7" ht="15.75">
       <c r="A143" s="42" t="s">
         <v>881</v>
       </c>
@@ -27236,7 +27246,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="15.5">
+    <row r="144" spans="1:7" ht="15.75">
       <c r="A144" s="42" t="s">
         <v>887</v>
       </c>
@@ -27259,7 +27269,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="15.5">
+    <row r="145" spans="1:7" ht="15.75">
       <c r="A145" s="42" t="s">
         <v>893</v>
       </c>
@@ -27282,7 +27292,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="15.5">
+    <row r="146" spans="1:7" ht="15.75">
       <c r="A146" s="42" t="s">
         <v>899</v>
       </c>
@@ -27305,7 +27315,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="15.5">
+    <row r="147" spans="1:7" ht="15.75">
       <c r="A147" s="42" t="s">
         <v>905</v>
       </c>
@@ -27328,7 +27338,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="15.5">
+    <row r="148" spans="1:7" ht="15.75">
       <c r="A148" s="42" t="s">
         <v>912</v>
       </c>
@@ -27351,7 +27361,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="15.5">
+    <row r="149" spans="1:7" ht="15.75">
       <c r="A149" s="42" t="s">
         <v>918</v>
       </c>
@@ -27374,7 +27384,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="15.5">
+    <row r="150" spans="1:7" ht="15.75">
       <c r="A150" s="42" t="s">
         <v>924</v>
       </c>
@@ -27397,7 +27407,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="15.5">
+    <row r="151" spans="1:7" ht="15.75">
       <c r="A151" s="42" t="s">
         <v>930</v>
       </c>
@@ -27420,7 +27430,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="15.5">
+    <row r="152" spans="1:7" ht="15.75">
       <c r="A152" s="42" t="s">
         <v>936</v>
       </c>
@@ -27443,7 +27453,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="15.5">
+    <row r="153" spans="1:7" ht="15.75">
       <c r="A153" s="42" t="s">
         <v>942</v>
       </c>
@@ -27466,7 +27476,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="15.5">
+    <row r="154" spans="1:7" ht="15.75">
       <c r="A154" s="42" t="s">
         <v>948</v>
       </c>
@@ -27489,7 +27499,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="15.5">
+    <row r="155" spans="1:7" ht="15.75">
       <c r="A155" s="42" t="s">
         <v>953</v>
       </c>
@@ -27512,7 +27522,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="15.5">
+    <row r="156" spans="1:7" ht="15.75">
       <c r="A156" s="42" t="s">
         <v>959</v>
       </c>
@@ -27535,7 +27545,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="15.5">
+    <row r="157" spans="1:7" ht="15.75">
       <c r="A157" s="42" t="s">
         <v>965</v>
       </c>
@@ -27558,7 +27568,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="15.5">
+    <row r="158" spans="1:7" ht="15.75">
       <c r="A158" s="42" t="s">
         <v>970</v>
       </c>
@@ -27581,7 +27591,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="15.5">
+    <row r="159" spans="1:7" ht="15.75">
       <c r="A159" s="42" t="s">
         <v>975</v>
       </c>
@@ -27604,7 +27614,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="15.5">
+    <row r="160" spans="1:7" ht="15.75">
       <c r="A160" s="42" t="s">
         <v>980</v>
       </c>
@@ -27627,7 +27637,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="15.5">
+    <row r="161" spans="1:7" ht="15.75">
       <c r="A161" s="42" t="s">
         <v>985</v>
       </c>
@@ -27650,7 +27660,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="15.5">
+    <row r="162" spans="1:7" ht="15.75">
       <c r="A162" s="42" t="s">
         <v>991</v>
       </c>
@@ -27673,7 +27683,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="15.5">
+    <row r="163" spans="1:7" ht="15.75">
       <c r="A163" s="42" t="s">
         <v>997</v>
       </c>
@@ -27696,7 +27706,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="15.5">
+    <row r="164" spans="1:7" ht="15.75">
       <c r="A164" s="42" t="s">
         <v>1003</v>
       </c>
@@ -27719,7 +27729,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="15.5">
+    <row r="165" spans="1:7" ht="15.75">
       <c r="A165" s="42" t="s">
         <v>1009</v>
       </c>
@@ -27742,7 +27752,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="15.5">
+    <row r="166" spans="1:7" ht="15.75">
       <c r="A166" s="42" t="s">
         <v>1014</v>
       </c>
@@ -27765,7 +27775,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="15.5">
+    <row r="167" spans="1:7" ht="15.75">
       <c r="A167" s="42" t="s">
         <v>1019</v>
       </c>
@@ -27788,7 +27798,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="15.5">
+    <row r="168" spans="1:7" ht="15.75">
       <c r="A168" s="42" t="s">
         <v>1025</v>
       </c>
@@ -27811,7 +27821,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="15.5">
+    <row r="169" spans="1:7" ht="15.75">
       <c r="A169" s="42" t="s">
         <v>1031</v>
       </c>
@@ -27834,7 +27844,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="15.5">
+    <row r="170" spans="1:7" ht="15.75">
       <c r="A170" s="42" t="s">
         <v>1036</v>
       </c>
@@ -27857,7 +27867,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="15.5">
+    <row r="171" spans="1:7" ht="15.75">
       <c r="A171" s="42" t="s">
         <v>1041</v>
       </c>
@@ -27880,7 +27890,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="15.5">
+    <row r="172" spans="1:7" ht="15.75">
       <c r="A172" s="42" t="s">
         <v>1046</v>
       </c>
@@ -27903,7 +27913,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="15.5">
+    <row r="173" spans="1:7" ht="15.75">
       <c r="A173" s="42" t="s">
         <v>1051</v>
       </c>
@@ -27926,7 +27936,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="15.5">
+    <row r="174" spans="1:7" ht="15.75">
       <c r="A174" s="42" t="s">
         <v>1058</v>
       </c>
@@ -27949,7 +27959,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="15.5">
+    <row r="175" spans="1:7" ht="15.75">
       <c r="A175" s="42" t="s">
         <v>1065</v>
       </c>
@@ -27972,7 +27982,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="15.5">
+    <row r="176" spans="1:7" ht="15.75">
       <c r="A176" s="42" t="s">
         <v>1071</v>
       </c>
@@ -27995,7 +28005,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="15.5">
+    <row r="177" spans="1:7" ht="15.75">
       <c r="A177" s="42" t="s">
         <v>1077</v>
       </c>
@@ -28018,7 +28028,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="15.5">
+    <row r="178" spans="1:7" ht="15.75">
       <c r="A178" s="42" t="s">
         <v>1083</v>
       </c>
@@ -28041,7 +28051,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="15.5">
+    <row r="179" spans="1:7" ht="15.75">
       <c r="A179" s="42" t="s">
         <v>1090</v>
       </c>
@@ -28064,7 +28074,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="15.5">
+    <row r="180" spans="1:7" ht="15.75">
       <c r="A180" s="42" t="s">
         <v>1097</v>
       </c>
@@ -28087,7 +28097,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="15.5">
+    <row r="181" spans="1:7" ht="15.75">
       <c r="A181" s="42" t="s">
         <v>1103</v>
       </c>
@@ -28110,7 +28120,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="15.5">
+    <row r="182" spans="1:7" ht="15.75">
       <c r="A182" s="42" t="s">
         <v>1109</v>
       </c>
@@ -28133,7 +28143,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="15.5">
+    <row r="183" spans="1:7" ht="15.75">
       <c r="A183" s="42" t="s">
         <v>1114</v>
       </c>
@@ -28352,13 +28362,13 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.81640625" defaultRowHeight="15.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15.6" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="41.453125" style="4" customWidth="1"/>
-    <col min="3" max="5" width="16.1796875" style="3" customWidth="1"/>
-    <col min="6" max="7" width="9.1796875" style="3"/>
-    <col min="8" max="16384" width="14.81640625" style="3"/>
+    <col min="1" max="1" width="16.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" style="4" customWidth="1"/>
+    <col min="3" max="5" width="16.140625" style="3" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="3"/>
+    <col min="8" max="16384" width="14.85546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
@@ -28375,7 +28385,7 @@
       <c r="E1" s="64"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="1" t="s">
         <v>1122</v>
       </c>
@@ -28387,7 +28397,7 @@
       <c r="E2" s="67"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="1" t="s">
         <v>1124</v>
       </c>
@@ -28478,7 +28488,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="15">
       <c r="A13" s="1" t="s">
         <v>1145</v>
       </c>
@@ -28542,7 +28552,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="15">
       <c r="A21" s="1" t="s">
         <v>1161</v>
       </c>
@@ -30432,27 +30442,27 @@
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.36328125" defaultRowHeight="15.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.6" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="61" customWidth="1"/>
-    <col min="2" max="2" width="11.36328125" customWidth="1"/>
-    <col min="3" max="7" width="9.1796875"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="7" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="14.5">
+    <row r="1" spans="1:1" ht="15">
       <c r="A1" s="8" t="s">
         <v>1629</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" ht="15">
       <c r="A2" s="9" t="s">
         <v>1630</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14.5">
+    <row r="3" spans="1:1" ht="15">
       <c r="A3" s="10"/>
     </row>
-    <row r="4" spans="1:1" ht="170.5">
+    <row r="4" spans="1:1" ht="165.75">
       <c r="A4" s="11" t="s">
         <v>1631</v>
       </c>
@@ -30474,15 +30484,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D364DC965387FD4EAF4833DDCF640F91" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c7401bc8bddc44f3d87e6545050f3282">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="18390984-f7d9-4502-80ba-82ec344db5fb" xmlns:ns3="629dd2dc-abea-47e8-ba88-82202e3ee8ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fc3cb6a02f8baa81433631181c409fee" ns2:_="" ns3:_="">
     <xsd:import namespace="18390984-f7d9-4502-80ba-82ec344db5fb"/>
@@ -30719,6 +30720,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -30731,14 +30741,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EBE091B-C892-47B3-9F2A-5DA83D5D54B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03260FC4-D767-4067-AFD9-7FD8DA82EDB7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30757,6 +30759,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EBE091B-C892-47B3-9F2A-5DA83D5D54B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBF2D27B-F605-4F88-8862-5E3188DD9C6A}">
   <ds:schemaRefs>

</xml_diff>